<commit_message>
change some config and optimization
</commit_message>
<xml_diff>
--- a/doc/RCL 等级对应可建造建筑.xlsx
+++ b/doc/RCL 等级对应可建造建筑.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MusicBear\Documents\GitHub\Screeps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub Repositories\Screeps\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C135A493-0D0D-43E4-9342-8A66B29F9DC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9808C6B-28AB-43B4-8072-B200F2D5322E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>RCL</t>
   </si>
@@ -120,6 +121,95 @@
   <si>
     <t>Other New Constructions</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挖矿所需时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级所需时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道路（空）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道路（满）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平原（空）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平原（满）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沼泽（空）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沼泽（满）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运输1格时间成本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平原</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沼泽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[MOVE,MOVE,WORK,CARRY]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[MOVE,WORK,CARRY]</t>
+  </si>
+  <si>
+    <t>[MOVE,WORK,WORK,CARRY]</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WORK时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOVE时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[MOVE,WORK,CARRY,CARRY]</t>
   </si>
 </sst>
 </file>
@@ -206,11 +296,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -223,9 +310,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -520,320 +629,324 @@
     <col min="7" max="7" width="5.875" customWidth="1"/>
     <col min="8" max="8" width="4.5" customWidth="1"/>
     <col min="9" max="9" width="4.25" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
         <v>200</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>45000</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>50</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>135000</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>405000</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1215000</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
         <v>30</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>50</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>2</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>3645000</v>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <v>40</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>50</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>2</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>3</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>10935000</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>100</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>4</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>6</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>60</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>200</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>6</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>6</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>10</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -842,4 +955,833 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80721B9C-7C4D-48C3-8A85-08934ECE8003}">
+  <dimension ref="A1:Q58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="7" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.625" customWidth="1"/>
+    <col min="10" max="10" width="11.625" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="13.125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>200</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>100</v>
+      </c>
+      <c r="F3" s="8">
+        <v>200</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2</v>
+      </c>
+      <c r="K3" s="9">
+        <v>5</v>
+      </c>
+      <c r="L3" s="9">
+        <v>10</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="9">
+        <f>E3+F3</f>
+        <v>300</v>
+      </c>
+      <c r="Q3" s="9" t="str">
+        <f>(G3+H3)&amp;TEXT(M3,"")&amp;"+"&amp;(I3+J3)&amp;TEXT(N3,"")&amp;"+"&amp;(K3+L3)&amp;TEXT(O3,"")</f>
+        <v>2x+3y+15z</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9">
+        <v>250</v>
+      </c>
+      <c r="E4" s="9">
+        <v>100</v>
+      </c>
+      <c r="F4" s="9">
+        <v>200</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1</v>
+      </c>
+      <c r="K4" s="9">
+        <v>3</v>
+      </c>
+      <c r="L4" s="9">
+        <v>5</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" ref="P4:P6" si="0">E4+F4</f>
+        <v>300</v>
+      </c>
+      <c r="Q4" s="9" t="str">
+        <f t="shared" ref="Q4:Q6" si="1">(G4+H4)&amp;TEXT(M4,"")&amp;"+"&amp;(I4+J4)&amp;TEXT(N4,"")&amp;"+"&amp;(K4+L4)&amp;TEXT(O4,"")</f>
+        <v>2x+2y+8z</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="9">
+        <v>250</v>
+      </c>
+      <c r="E5" s="9">
+        <v>100</v>
+      </c>
+      <c r="F5" s="9">
+        <v>200</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9">
+        <v>5</v>
+      </c>
+      <c r="L5" s="9">
+        <v>15</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="Q5" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>3x+4y+20z</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="9">
+        <v>300</v>
+      </c>
+      <c r="E6" s="9">
+        <f>13*4</f>
+        <v>52</v>
+      </c>
+      <c r="F6" s="9">
+        <f>25*4</f>
+        <v>100</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9">
+        <v>10</v>
+      </c>
+      <c r="L6" s="9">
+        <v>15</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="Q6" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>3x+5y+25z</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>